<commit_message>
Code Fixes and Retry Addition
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestClssSecond.xlsx
+++ b/src/test/resources/excel/TestClssSecond.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>first</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>two</t>
+  </si>
+  <si>
+    <t>one</t>
   </si>
 </sst>
 </file>
@@ -365,7 +368,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,7 +386,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Data Provider Complete fix
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestClssSecond.xlsx
+++ b/src/test/resources/excel/TestClssSecond.xlsx
@@ -24,20 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>first</t>
   </si>
   <si>
-    <t>second</t>
-  </si>
-  <si>
-    <t>third</t>
-  </si>
-  <si>
-    <t>bricks</t>
-  </si>
-  <si>
     <t>pappu</t>
   </si>
   <si>
@@ -47,7 +38,25 @@
     <t>two</t>
   </si>
   <si>
-    <t>one</t>
+    <t>last</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>dabbu</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>three</t>
+  </si>
+  <si>
+    <t>dahakan</t>
+  </si>
+  <si>
+    <t>NY</t>
   </si>
 </sst>
 </file>
@@ -365,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -378,32 +387,43 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>